<commit_message>
MOD: change heder posision on sheet2
</commit_message>
<xml_diff>
--- a/test/data/test_book.xlsx
+++ b/test/data/test_book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>#</t>
     <phoneticPr fontId="2"/>
@@ -159,6 +159,10 @@
   </si>
   <si>
     <t>…</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Sone explanations…</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -278,17 +282,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -622,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -634,31 +639,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
@@ -676,121 +681,121 @@
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="4" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="4" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -809,10 +814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -823,120 +828,125 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="4" spans="2:12">
-      <c r="B4" s="2" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1">
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
-      <c r="B5" s="4">
+    <row r="6" spans="2:12">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="4" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="2:12">
-      <c r="B6" s="4">
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>